<commit_message>
Update project questions and word document
</commit_message>
<xml_diff>
--- a/Correlation.xlsx
+++ b/Correlation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Koutn\sql-repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C851C9F-6B9E-4F9F-8EAE-0E24124ABC17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{584046CB-BBE0-46F8-9CC8-4F74FA1931D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59,10 +59,10 @@
     <t>Souvislost mezi růstem mezd a HDP ve stejném roce</t>
   </si>
   <si>
-    <t>Souvislost mezi růstem mezd v následujícím roce a HDP ve předchozím roce</t>
+    <t>Korelačni koeficient mezi růstem mezd a HDP pouze pro HDP &gt; 5%</t>
   </si>
   <si>
-    <t>Korelačni koeficient mezi růstem mezd a HDP pouze pro HDP &gt; 5%</t>
+    <t>Souvislost mezi růstem mezd v roce x+1 a HDP v roce x</t>
   </si>
 </sst>
 </file>
@@ -617,9 +617,7 @@
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1025,16 +1023,16 @@
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
-      <c r="H1" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
+      <c r="H1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
       <c r="M1" s="7"/>
       <c r="P1" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Q1" s="6"/>
       <c r="R1" s="6"/>
@@ -1410,7 +1408,7 @@
         <v>2009</v>
       </c>
       <c r="P12" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Q12" s="6"/>
       <c r="R12" s="6"/>
@@ -1784,9 +1782,9 @@
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:E1"/>
-    <mergeCell ref="H1:M1"/>
     <mergeCell ref="P1:U1"/>
     <mergeCell ref="P12:U12"/>
+    <mergeCell ref="H1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>